<commit_message>
added carousel to todo panel and updated map page infowindows
</commit_message>
<xml_diff>
--- a/sql/markers.xlsx
+++ b/sql/markers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="100">
   <si>
     <t>Category</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>http://www.cafebeignet.com/</t>
   </si>
 </sst>
 </file>
@@ -675,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,6 +1074,9 @@
       <c r="D16" t="s">
         <v>64</v>
       </c>
+      <c r="E16" t="s">
+        <v>99</v>
+      </c>
       <c r="G16">
         <v>29.955226</v>
       </c>
@@ -1266,6 +1272,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E16" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1274,7 +1283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated todo panel layout and text
</commit_message>
<xml_diff>
--- a/sql/markers.xlsx
+++ b/sql/markers.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="136">
   <si>
     <t>Category</t>
   </si>
@@ -120,9 +120,6 @@
     <t>http://www.pizzadomenica.com/</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/place/PIZZA+domenica/@29.9204938,-90.1088353,15z/data=!4m5!3m4!1s0x0:0xea94fab39a45b76d!8m2!3d29.9204938!4d-90.1088353</t>
-  </si>
-  <si>
     <t>Seaworthy</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>http://www.seaworthynola.com/</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/place/SEAWORTHY/@29.947879,-90.072208,15z/data=!4m5!3m4!1s0x0:0x1a15023dd6c1e365!8m2!3d29.947879!4d-90.072208</t>
-  </si>
-  <si>
     <t>Drinks</t>
   </si>
   <si>
@@ -147,9 +141,6 @@
     <t>http://hotelmonteleone.com/entertainment/carousel-bar/</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/place/Carousel+Bar/@29.954163,-90.068029,15z/data=!4m2!3m1!1s0x0:0xdd909df48675434d?sa=X&amp;ved=0ahUKEwiY-cPQuYvSAhXDZiYKHa2SC8kQ_BIIjAEwDg</t>
-  </si>
-  <si>
     <t>Arnuad's French 75</t>
   </si>
   <si>
@@ -159,9 +150,6 @@
     <t>https://www.arnaudsrestaurant.com/bars/french-75/</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/place/French+75/@29.9557933,-90.0686926,15z/data=!4m5!3m4!1s0x0:0xbbb24fa3f0588a4c!8m2!3d29.9557933!4d-90.0686926</t>
-  </si>
-  <si>
     <t>Erin Rose</t>
   </si>
   <si>
@@ -183,9 +171,6 @@
     <t>http://hottinbar.com/</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/place/Hot+Tin/@29.9351131,-90.0797176,15z/data=!4m2!3m1!1s0x0:0xca107f3e51a95c55?sa=X&amp;ved=0ahUKEwju__qSuovSAhVBPCYKHWz9BpIQ_BIIhgEwCg</t>
-  </si>
-  <si>
     <t>Cure</t>
   </si>
   <si>
@@ -216,9 +201,6 @@
     <t>http://www.cafedumonde.com/</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/place/Cafe+Du+Monde/@29.9574643,-90.0618811,15z/data=!4m2!3m1!1s0x0:0xd68fe7e8e35b6f7?sa=X&amp;ved=0ahUKEwi-h8TCwovSAhVGTSYKHXxKCSwQ_BIIdzAN</t>
-  </si>
-  <si>
     <t>Cafe Beignet</t>
   </si>
   <si>
@@ -328,6 +310,132 @@
   </si>
   <si>
     <t>http://www.cafebeignet.com/</t>
+  </si>
+  <si>
+    <t>600 Poland Ave New Orleans, LA 70117</t>
+  </si>
+  <si>
+    <t>Bywater</t>
+  </si>
+  <si>
+    <t>Bacchanal Wine</t>
+  </si>
+  <si>
+    <t>Shaya</t>
+  </si>
+  <si>
+    <t>4213 Magazine St New Orleans, LA 70115</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>restaurant</t>
+  </si>
+  <si>
+    <t>description text Cafe Amelie</t>
+  </si>
+  <si>
+    <t>description text Sylvain</t>
+  </si>
+  <si>
+    <t>description text Cochon</t>
+  </si>
+  <si>
+    <t>description text Cochon Butcher</t>
+  </si>
+  <si>
+    <t>description text Coquette</t>
+  </si>
+  <si>
+    <t>description text Pizza Domenica</t>
+  </si>
+  <si>
+    <t>description text Seaworthy</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>description text Carousel Bar</t>
+  </si>
+  <si>
+    <t>description text Arnuad's French 75</t>
+  </si>
+  <si>
+    <t>description text Erin Rose</t>
+  </si>
+  <si>
+    <t>description text Hot Tin</t>
+  </si>
+  <si>
+    <t>description text Cure</t>
+  </si>
+  <si>
+    <t>description text The Avenue Pub</t>
+  </si>
+  <si>
+    <t>description text Cafe Du Monde</t>
+  </si>
+  <si>
+    <t>description text Cafe Beignet</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>description text Preservation Hall</t>
+  </si>
+  <si>
+    <t>description text Spotted Cat</t>
+  </si>
+  <si>
+    <t>description text dba</t>
+  </si>
+  <si>
+    <t>description text The National WWII Museum</t>
+  </si>
+  <si>
+    <t>hotel</t>
+  </si>
+  <si>
+    <t>description text Hotel Monteleone</t>
+  </si>
+  <si>
+    <t>description text Bienville House</t>
+  </si>
+  <si>
+    <t>description text Napoleon House</t>
+  </si>
+  <si>
+    <t>description text New Orleans Pharmacy Museum</t>
+  </si>
+  <si>
+    <t>venue</t>
+  </si>
+  <si>
+    <t>724 Iberville Street New Orleans, LA 70130</t>
+  </si>
+  <si>
+    <t>Acme Oyster House</t>
+  </si>
+  <si>
+    <t>tourist</t>
+  </si>
+  <si>
+    <t>718 St Peter St, New Orleans, LA 70116</t>
+  </si>
+  <si>
+    <t>Pat O'Brien's</t>
+  </si>
+  <si>
+    <t>http://www.patobriens.com/patobriens/default.asp</t>
+  </si>
+  <si>
+    <t>http://www.acmeoyster.com/</t>
   </si>
 </sst>
 </file>
@@ -676,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,10 +800,11 @@
     <col min="6" max="6" width="169.140625" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="176.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -720,8 +829,14 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -743,8 +858,14 @@
       <c r="H2">
         <v>-90.062984999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -766,8 +887,14 @@
       <c r="H3">
         <v>-90.064204000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -789,8 +916,14 @@
       <c r="H4">
         <v>-90.067122999999995</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -812,8 +945,14 @@
       <c r="H5">
         <v>-90.067122999999995</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -835,8 +974,14 @@
       <c r="H6">
         <v>-90.082465999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>101</v>
+      </c>
+      <c r="J6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -859,24 +1004,27 @@
         <v>-90.108834999999999</v>
       </c>
       <c r="I7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="J7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
       <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
         <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
       </c>
       <c r="G8">
         <v>29.947879</v>
@@ -885,24 +1033,27 @@
         <v>-90.072208000000003</v>
       </c>
       <c r="I8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G9">
         <v>29.954295999999999</v>
@@ -911,24 +1062,27 @@
         <v>-90.067786999999996</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="J9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G10">
         <v>29.955812000000002</v>
@@ -937,27 +1091,30 @@
         <v>-90.068702999999999</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="J10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G11">
         <v>29.956553</v>
@@ -965,22 +1122,28 @@
       <c r="H11">
         <v>-90.067937999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>109</v>
+      </c>
+      <c r="J11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G12">
         <v>29.935110999999999</v>
@@ -989,24 +1152,27 @@
         <v>-90.079721000000006</v>
       </c>
       <c r="I12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="J12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G13">
         <v>29.935023000000001</v>
@@ -1014,22 +1180,28 @@
       <c r="H13">
         <v>-90.107460000000003</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>109</v>
+      </c>
+      <c r="J13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
         <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G14">
         <v>29.936914999999999</v>
@@ -1037,22 +1209,28 @@
       <c r="H14">
         <v>-90.076750000000004</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>109</v>
+      </c>
+      <c r="J14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G15">
         <v>29.957464000000002</v>
@@ -1061,21 +1239,24 @@
         <v>-90.061881</v>
       </c>
       <c r="I15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="J15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
         <v>58</v>
       </c>
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" t="s">
-        <v>64</v>
-      </c>
       <c r="E16" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G16">
         <v>29.955226</v>
@@ -1083,25 +1264,31 @@
       <c r="H16">
         <v>-90.067079000000007</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>101</v>
+      </c>
+      <c r="J16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G17">
         <v>29.958300999999999</v>
@@ -1109,22 +1296,28 @@
       <c r="H17">
         <v>-90.065396000000007</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>118</v>
+      </c>
+      <c r="J17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
         <v>65</v>
       </c>
-      <c r="B18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" t="s">
-        <v>71</v>
-      </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E18" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G18">
         <v>29.964061000000001</v>
@@ -1132,22 +1325,28 @@
       <c r="H18">
         <v>-90.057666999999995</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>118</v>
+      </c>
+      <c r="J18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
         <v>65</v>
       </c>
-      <c r="B19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" t="s">
-        <v>71</v>
-      </c>
       <c r="D19" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G19">
         <v>29.963943</v>
@@ -1155,22 +1354,28 @@
       <c r="H19">
         <v>-90.058027999999993</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>118</v>
+      </c>
+      <c r="J19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G20">
         <v>29.943017999999999</v>
@@ -1178,22 +1383,28 @@
       <c r="H20">
         <v>-90.070106999999993</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>118</v>
+      </c>
+      <c r="J20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E21" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G21">
         <v>29.954295999999999</v>
@@ -1201,22 +1412,28 @@
       <c r="H21">
         <v>-90.067786999999996</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>123</v>
+      </c>
+      <c r="J21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G22">
         <v>29.953831000000001</v>
@@ -1224,22 +1441,28 @@
       <c r="H22">
         <v>-90.065279000000004</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>123</v>
+      </c>
+      <c r="J22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E23" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G23">
         <v>29.955878999999999</v>
@@ -1247,28 +1470,84 @@
       <c r="H23">
         <v>-90.065056999999996</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>128</v>
+      </c>
+      <c r="J23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E24" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G24">
         <v>29.956050999999999</v>
       </c>
       <c r="H24">
         <v>-90.064935000000006</v>
+      </c>
+      <c r="I24" t="s">
+        <v>128</v>
+      </c>
+      <c r="J24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" t="s">
+        <v>129</v>
+      </c>
+      <c r="E27" t="s">
+        <v>135</v>
+      </c>
+      <c r="I27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" t="s">
+        <v>132</v>
+      </c>
+      <c r="E28" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1298,19 +1577,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1420,10 +1699,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
         <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
       </c>
       <c r="D8">
         <v>29.947879</v>
@@ -1437,10 +1716,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9">
         <v>29.954295999999999</v>
@@ -1454,10 +1733,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D10">
         <v>29.955812000000002</v>
@@ -1471,10 +1750,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D11">
         <v>29.956553</v>
@@ -1488,10 +1767,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D12">
         <v>29.935110999999999</v>
@@ -1505,10 +1784,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D13">
         <v>29.935023000000001</v>
@@ -1522,10 +1801,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D14">
         <v>29.936914999999999</v>
@@ -1539,10 +1818,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D15">
         <v>29.957464000000002</v>
@@ -1556,10 +1835,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D16">
         <v>29.955226</v>
@@ -1573,10 +1852,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D17">
         <v>29.958300999999999</v>
@@ -1590,10 +1869,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D18">
         <v>29.964061000000001</v>
@@ -1607,10 +1886,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D19">
         <v>29.963943</v>
@@ -1624,10 +1903,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D20">
         <v>29.943017999999999</v>
@@ -1641,10 +1920,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D21">
         <v>29.954295999999999</v>
@@ -1658,10 +1937,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D22">
         <v>29.953831000000001</v>
@@ -1675,10 +1954,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D23">
         <v>29.955878999999999</v>
@@ -1692,10 +1971,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D24">
         <v>29.956050999999999</v>

</xml_diff>